<commit_message>
Data Visualization and Dashboards with Excel and Cognos
</commit_message>
<xml_diff>
--- a/2 - Excel/Final Project/Part 2/Montgomery_Fleet_Equipment_Inventory_FA_PART_2_START.xlsx
+++ b/2 - Excel/Final Project/Part 2/Montgomery_Fleet_Equipment_Inventory_FA_PART_2_START.xlsx
@@ -1,29 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\stevesstuff\Job_Stuff\Skill-UpTechnologies\IBM\DataAnalystCurriculumDesign\Course 2 - Analyzing &amp; Visualizing Data Using Spreadsheets\Labs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODES\IBM---Data-Analyst---Professinal-Certificate\2 - Excel\Final Project\Part 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9011A403-47E5-440B-B7E1-02326158FD21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA48EC1-07CE-44E6-A161-D0B0B3269D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Montgomery_Fleet_Equipment_Inve" sheetId="1" r:id="rId1"/>
+    <sheet name="Pivot 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Pivot 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Pivot 3" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Montgomery_Fleet_Equipment_Inve!$A$1:$C$50</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="16" r:id="rId5"/>
+  </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="38">
   <si>
     <t>Department</t>
   </si>
@@ -110,13 +125,40 @@
   </si>
   <si>
     <t>Off Road Vehicle Equipment</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>AVERAGE</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>COUNT</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of Equipment Count</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,8 +293,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -432,8 +480,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -548,6 +602,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -593,8 +677,28 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -651,6 +755,750 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Wasi" refreshedDate="44512.342763773151" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="49" xr:uid="{ADB3141A-C308-4C02-BAED-0B667712B990}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Table1"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Department" numFmtId="0">
+      <sharedItems count="12">
+        <s v="Housing and Community Affairs"/>
+        <s v="Human Rights"/>
+        <s v="Libraries"/>
+        <s v="Liquor Control"/>
+        <s v="Office Of Homeland Security"/>
+        <s v="Permitting Services"/>
+        <s v="Public Information Office"/>
+        <s v="Recreation"/>
+        <s v="Sheriffs Office"/>
+        <s v="State Attorneys Office"/>
+        <s v="Technology Services"/>
+        <s v="Transportation"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Equipment Class" numFmtId="0">
+      <sharedItems count="14">
+        <s v="Pick Up Trucks"/>
+        <s v="SUV"/>
+        <s v="Sedan"/>
+        <s v="Van"/>
+        <s v="Medium Duty"/>
+        <s v="Heavy Duty"/>
+        <s v="CUV"/>
+        <s v="Off Road Vehicle Equipment"/>
+        <s v="Public Safety SUV"/>
+        <s v="Public Safety Van"/>
+        <s v="Public Safety CUV"/>
+        <s v="Public Safety Sedan"/>
+        <s v="Public Safety Pick Up Trucks"/>
+        <s v="Transit Bus"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Equipment Count" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="379"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="49">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="21"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="23"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <n v="42"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="11"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="6"/>
+    <n v="9"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="27"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="24"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="48"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="2"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="3"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="7"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="8"/>
+    <n v="20"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="9"/>
+    <n v="8"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="10"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="11"/>
+    <n v="46"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="12"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="11"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="3"/>
+    <n v="11"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="0"/>
+    <n v="93"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="5"/>
+    <n v="248"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="13"/>
+    <n v="379"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="1"/>
+    <n v="53"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="3"/>
+    <n v="32"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="4"/>
+    <n v="98"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="7"/>
+    <n v="276"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="6"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="2"/>
+    <n v="37"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BDA2DEC4-B052-47CC-87FC-469E4BBF6240}" name="PivotTable3" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:P15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="13">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
+      <items count="15">
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item x="0"/>
+        <item x="10"/>
+        <item x="12"/>
+        <item x="11"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="13"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="13">
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="15">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Equipment Count" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{75FD25A7-90B4-464E-85E8-B4BD7F6AE4A2}" name="PivotTable4" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:B23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="13">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="15">
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item x="0"/>
+        <item x="10"/>
+        <item x="12"/>
+        <item x="11"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="13"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="22">
+    <i>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Equipment Count" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{41CAE3C9-7353-460C-BFDE-C2DE231CB79A}" name="PivotTable5" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:B19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="13">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="15">
+        <item x="6"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="13"/>
+        <item sd="0" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="18">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Equipment Count" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ACD81276-67D3-43D8-A805-4BF8391E155C}" name="Table1" displayName="Table1" ref="A1:C50" totalsRowShown="0">
+  <autoFilter ref="A1:C50" xr:uid="{ACD81276-67D3-43D8-A805-4BF8391E155C}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{BAF1A8A3-D1E1-4577-BE67-C15128D57BE8}" name="Department"/>
+    <tableColumn id="2" xr3:uid="{EB1F7AB4-B789-41EB-B0D3-864CF8446BA2}" name="Equipment Class"/>
+    <tableColumn id="3" xr3:uid="{287CC09A-C487-4915-BC73-2C50A64830EF}" name="Equipment Count"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -949,19 +1797,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C50"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="33" width="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -972,7 +1843,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -982,8 +1853,15 @@
       <c r="C2">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="2">
+        <f>SUBTOTAL(109,C2:C50)</f>
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -993,8 +1871,15 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="1">
+        <f>SUBTOTAL(101,C2:C50)</f>
+        <v>32.285714285714285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1004,8 +1889,15 @@
       <c r="C4">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="2">
+        <f>SUBTOTAL(105,C2:C50)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1015,8 +1907,15 @@
       <c r="C5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="1">
+        <f>SUBTOTAL(109,C2:C50)</f>
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1026,8 +1925,15 @@
       <c r="C6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="3">
+        <f>SUBTOTAL(102,C2:C50)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1038,7 +1944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1049,7 +1955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1060,7 +1966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1071,7 +1977,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1082,7 +1988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1093,7 +1999,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1104,7 +2010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1115,7 +2021,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1126,7 +2032,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1509,6 +2415,915 @@
       </c>
       <c r="C50">
         <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{185E3BB3-40FA-4EF7-B29B-A02BBA9460E8}">
+  <dimension ref="A1:P15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="9">
+        <v>5</v>
+      </c>
+      <c r="C3" s="9">
+        <v>248</v>
+      </c>
+      <c r="D3" s="9">
+        <v>98</v>
+      </c>
+      <c r="E3" s="9">
+        <v>276</v>
+      </c>
+      <c r="F3" s="9">
+        <v>93</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9">
+        <v>37</v>
+      </c>
+      <c r="M3" s="9">
+        <v>53</v>
+      </c>
+      <c r="N3" s="9">
+        <v>379</v>
+      </c>
+      <c r="O3" s="9">
+        <v>32</v>
+      </c>
+      <c r="P3" s="9">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="9">
+        <v>9</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9">
+        <v>24</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9">
+        <v>48</v>
+      </c>
+      <c r="M4" s="9">
+        <v>27</v>
+      </c>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9">
+        <v>1</v>
+      </c>
+      <c r="P4" s="9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9">
+        <v>3</v>
+      </c>
+      <c r="G5" s="9">
+        <v>4</v>
+      </c>
+      <c r="H5" s="9">
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
+        <v>46</v>
+      </c>
+      <c r="J5" s="9">
+        <v>20</v>
+      </c>
+      <c r="K5" s="9">
+        <v>8</v>
+      </c>
+      <c r="L5" s="9">
+        <v>1</v>
+      </c>
+      <c r="M5" s="9">
+        <v>1</v>
+      </c>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9">
+        <v>42</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9">
+        <v>11</v>
+      </c>
+      <c r="M6" s="9">
+        <v>1</v>
+      </c>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9">
+        <v>2</v>
+      </c>
+      <c r="P6" s="9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9">
+        <v>21</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9">
+        <v>23</v>
+      </c>
+      <c r="M7" s="9">
+        <v>1</v>
+      </c>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9">
+        <v>7</v>
+      </c>
+      <c r="F8" s="9">
+        <v>5</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9">
+        <v>6</v>
+      </c>
+      <c r="M8" s="9">
+        <v>2</v>
+      </c>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9">
+        <v>15</v>
+      </c>
+      <c r="P8" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9">
+        <v>3</v>
+      </c>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9">
+        <v>11</v>
+      </c>
+      <c r="P9" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9">
+        <v>1</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9">
+        <v>3</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9">
+        <v>2</v>
+      </c>
+      <c r="P10" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9">
+        <v>1</v>
+      </c>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9">
+        <v>2</v>
+      </c>
+      <c r="M11" s="9">
+        <v>1</v>
+      </c>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9">
+        <v>1</v>
+      </c>
+      <c r="P11" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9">
+        <v>2</v>
+      </c>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9">
+        <v>1</v>
+      </c>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9">
+        <v>1</v>
+      </c>
+      <c r="P14" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="9">
+        <v>15</v>
+      </c>
+      <c r="C15" s="9">
+        <v>290</v>
+      </c>
+      <c r="D15" s="9">
+        <v>100</v>
+      </c>
+      <c r="E15" s="9">
+        <v>283</v>
+      </c>
+      <c r="F15" s="9">
+        <v>150</v>
+      </c>
+      <c r="G15" s="9">
+        <v>4</v>
+      </c>
+      <c r="H15" s="9">
+        <v>1</v>
+      </c>
+      <c r="I15" s="9">
+        <v>47</v>
+      </c>
+      <c r="J15" s="9">
+        <v>20</v>
+      </c>
+      <c r="K15" s="9">
+        <v>8</v>
+      </c>
+      <c r="L15" s="9">
+        <v>130</v>
+      </c>
+      <c r="M15" s="9">
+        <v>90</v>
+      </c>
+      <c r="N15" s="9">
+        <v>379</v>
+      </c>
+      <c r="O15" s="9">
+        <v>65</v>
+      </c>
+      <c r="P15" s="9">
+        <v>1582</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0045D82-E517-43C6-9F20-6C314C788DAD}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="9">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="9">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="9">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="9">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="9">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="9">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="9">
+        <v>1582</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD5A66D-2CB2-4FC6-B304-92CC4E8D1019}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="9">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="9">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="9">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="9">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="9">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="9">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="9">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="9">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="9">
+        <v>1582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>